<commit_message>
configs and minor changes
</commit_message>
<xml_diff>
--- a/New Terminals/Scripts/ConversãoDataCDC.xlsx
+++ b/New Terminals/Scripts/ConversãoDataCDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\New Terminals\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAB74C5F-5C37-4F5E-870E-1D053A4B4707}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBE752A-2317-4EAE-B69D-C94BFFA1B689}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="5085" yWindow="4905" windowWidth="21600" windowHeight="11040" xr2:uid="{B052DA09-9D1F-47DC-9B08-88E6AD2BA9C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B052DA09-9D1F-47DC-9B08-88E6AD2BA9C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Data &lt;-&gt; CDC" sheetId="2" r:id="rId1"/>
@@ -521,7 +521,7 @@
   <dimension ref="B2:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,18 +578,18 @@
     </row>
     <row r="5" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B5" s="2">
-        <v>44517</v>
+        <v>44533</v>
       </c>
       <c r="C5" s="4">
         <f t="shared" ref="C5:C10" si="1">IF(B5 &gt;= DATE(2001,5,1), B5-DATE(2001,5,1)+1,"Data inválida")</f>
-        <v>7506</v>
+        <v>7522</v>
       </c>
       <c r="E5" s="3">
-        <v>7491</v>
+        <v>7534</v>
       </c>
       <c r="F5" s="6">
-        <f t="shared" si="0"/>
-        <v>44502</v>
+        <f>IF(E5 &gt; 0, DATE(2001,5,1)+E5-1, "cdc inválido")</f>
+        <v>44545</v>
       </c>
     </row>
     <row r="6" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
log files of the rotation of the day in Millennium system.
</commit_message>
<xml_diff>
--- a/New Terminals/Scripts/ConversãoDataCDC.xlsx
+++ b/New Terminals/Scripts/ConversãoDataCDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\New Terminals\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DBE752A-2317-4EAE-B69D-C94BFFA1B689}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871E99C4-BA41-4D80-8435-BD46158D47E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B052DA09-9D1F-47DC-9B08-88E6AD2BA9C1}"/>
+    <workbookView xWindow="4455" yWindow="4335" windowWidth="21600" windowHeight="11265" tabRatio="541" xr2:uid="{B052DA09-9D1F-47DC-9B08-88E6AD2BA9C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Data &lt;-&gt; CDC" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>NOTA: a data CDC começou a contar no dia 01 de maio de 2001</t>
   </si>
@@ -87,11 +87,20 @@
       <t xml:space="preserve"> Data</t>
     </r>
   </si>
+  <si>
+    <t>rep</t>
+  </si>
+  <si>
+    <t>prg</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="ddd\ dd/mm/yyyy"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -133,7 +142,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -143,6 +152,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -174,14 +195,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -191,9 +209,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -201,9 +216,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -518,153 +542,178 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4918C6DD-70F1-489F-A28A-CFD3A071513C}">
-  <dimension ref="B2:G12"/>
+  <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="12.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="4.42578125" customWidth="1"/>
     <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="E2" s="10" t="s">
+      <c r="C2" s="12"/>
+      <c r="E2" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="10"/>
-    </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B3" s="2">
+      <c r="F2" s="12"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B3" s="9">
         <v>36535</v>
       </c>
-      <c r="C3" s="4" t="str">
+      <c r="C3" s="3" t="str">
         <f>IF(B3 &gt;= DATE(2001,5,1), B3-DATE(2001,5,1)+1,"Data inválida")</f>
         <v>Data inválida</v>
       </c>
-      <c r="E3" s="3">
+      <c r="E3" s="2">
         <v>1</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="8">
         <f>IF(E3 &gt; 0, DATE(2001,5,1)+E3-1, "cdc inválido")</f>
         <v>37012</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
-        <v>44505</v>
-      </c>
-      <c r="C4" s="4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="9">
+        <v>44628</v>
+      </c>
+      <c r="C4" s="3">
         <f>IF(B4 &gt;= DATE(2001,5,1), B4-DATE(2001,5,1)+1,"Data inválida")</f>
-        <v>7494</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0</v>
-      </c>
-      <c r="F4" s="6" t="str">
+        <v>7617</v>
+      </c>
+      <c r="E4" s="2">
+        <v>7617</v>
+      </c>
+      <c r="F4" s="8">
         <f t="shared" ref="F4:F10" si="0">IF(E4 &gt; 0, DATE(2001,5,1)+E4-1, "cdc inválido")</f>
-        <v>cdc inválido</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B5" s="2">
-        <v>44533</v>
-      </c>
-      <c r="C5" s="4">
+        <v>44628</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5" s="9">
+        <v>44622</v>
+      </c>
+      <c r="C5" s="3">
         <f t="shared" ref="C5:C10" si="1">IF(B5 &gt;= DATE(2001,5,1), B5-DATE(2001,5,1)+1,"Data inválida")</f>
-        <v>7522</v>
-      </c>
-      <c r="E5" s="3">
-        <v>7534</v>
-      </c>
-      <c r="F5" s="6">
+        <v>7611</v>
+      </c>
+      <c r="E5" s="2">
+        <v>7528</v>
+      </c>
+      <c r="F5" s="8">
         <f>IF(E5 &gt; 0, DATE(2001,5,1)+E5-1, "cdc inválido")</f>
-        <v>44545</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="2"/>
-      <c r="C6" s="4" t="str">
+        <v>44539</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9">
+        <v>44623</v>
+      </c>
+      <c r="C6" s="3">
+        <f t="shared" si="1"/>
+        <v>7612</v>
+      </c>
+      <c r="E6" s="2">
+        <v>7600</v>
+      </c>
+      <c r="F6" s="8">
+        <f t="shared" si="0"/>
+        <v>44611</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="9">
+        <v>44497</v>
+      </c>
+      <c r="C7" s="3">
+        <f t="shared" si="1"/>
+        <v>7486</v>
+      </c>
+      <c r="E7" s="2">
+        <v>7610</v>
+      </c>
+      <c r="F7" s="8">
+        <f t="shared" si="0"/>
+        <v>44621</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8" s="9">
+        <v>44502</v>
+      </c>
+      <c r="C8" s="3">
+        <f t="shared" si="1"/>
+        <v>7491</v>
+      </c>
+      <c r="E8" s="2">
+        <v>7493</v>
+      </c>
+      <c r="F8" s="8">
+        <f t="shared" si="0"/>
+        <v>44504</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9" s="9">
+        <v>44539</v>
+      </c>
+      <c r="C9" s="3">
+        <f t="shared" si="1"/>
+        <v>7528</v>
+      </c>
+      <c r="E9" s="2">
+        <v>7491</v>
+      </c>
+      <c r="F9" s="8">
+        <f t="shared" si="0"/>
+        <v>44502</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="9"/>
+      <c r="C10" s="3" t="str">
         <f t="shared" si="1"/>
         <v>Data inválida</v>
       </c>
-      <c r="E6" s="3"/>
-      <c r="F6" s="6" t="str">
+      <c r="E10" s="2">
+        <v>7525</v>
+      </c>
+      <c r="F10" s="8">
         <f t="shared" si="0"/>
-        <v>cdc inválido</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="2"/>
-      <c r="C7" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Data inválida</v>
-      </c>
-      <c r="E7" s="3"/>
-      <c r="F7" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>cdc inválido</v>
-      </c>
-    </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Data inválida</v>
-      </c>
-      <c r="E8" s="3"/>
-      <c r="F8" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>cdc inválido</v>
-      </c>
-    </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B9" s="2"/>
-      <c r="C9" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Data inválida</v>
-      </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>cdc inválido</v>
-      </c>
-    </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="4" t="str">
-        <f t="shared" si="1"/>
-        <v>Data inválida</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="6" t="str">
-        <f t="shared" si="0"/>
-        <v>cdc inválido</v>
-      </c>
-    </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
+        <v>44536</v>
+      </c>
+      <c r="G10" s="11"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
       <c r="C11"/>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B12" s="7" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="9"/>
-      <c r="F12" s="9"/>
-      <c r="G12" s="9"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="7"/>
+      <c r="E12" s="7"/>
+      <c r="F12" s="7"/>
+      <c r="G12" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
documentation about MessageQ and Analyse about the IPS list of establishement/orderNum ready for Reception and Action for the Hades automation testes.
Former-commit-id: 224ddb1726f83f37547a291162130d4a52f28a95
</commit_message>
<xml_diff>
--- a/New Terminals/Scripts/ConversãoDataCDC.xlsx
+++ b/New Terminals/Scripts/ConversãoDataCDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\New Terminals\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{871E99C4-BA41-4D80-8435-BD46158D47E6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0069E51C-765F-4436-BE75-8786882E55D4}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4455" yWindow="4335" windowWidth="21600" windowHeight="11265" tabRatio="541" xr2:uid="{B052DA09-9D1F-47DC-9B08-88E6AD2BA9C1}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="541" xr2:uid="{B052DA09-9D1F-47DC-9B08-88E6AD2BA9C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Data &lt;-&gt; CDC" sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>NOTA: a data CDC começou a contar no dia 01 de maio de 2001</t>
   </si>
@@ -93,6 +93,12 @@
   <si>
     <t>prg</t>
   </si>
+  <si>
+    <t>IPS</t>
+  </si>
+  <si>
+    <t>MILL</t>
+  </si>
 </sst>
 </file>
 
@@ -142,7 +148,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +170,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -195,7 +213,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -224,10 +242,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -545,7 +565,7 @@
   <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -559,14 +579,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="E2" s="12" t="s">
+      <c r="C2" s="15"/>
+      <c r="E2" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="12"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="9">
@@ -585,7 +605,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="12" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="9">
@@ -656,11 +676,11 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8" s="9">
-        <v>44502</v>
+        <v>44659</v>
       </c>
       <c r="C8" s="3">
         <f t="shared" si="1"/>
-        <v>7491</v>
+        <v>7648</v>
       </c>
       <c r="E8" s="2">
         <v>7493</v>
@@ -671,12 +691,15 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>6</v>
+      </c>
       <c r="B9" s="9">
-        <v>44539</v>
+        <v>44656</v>
       </c>
       <c r="C9" s="3">
         <f t="shared" si="1"/>
-        <v>7528</v>
+        <v>7645</v>
       </c>
       <c r="E9" s="2">
         <v>7491</v>
@@ -687,10 +710,15 @@
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B10" s="9"/>
-      <c r="C10" s="3" t="str">
+      <c r="A10" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="9">
+        <v>44592</v>
+      </c>
+      <c r="C10" s="3">
         <f t="shared" si="1"/>
-        <v>Data inválida</v>
+        <v>7581</v>
       </c>
       <c r="E10" s="2">
         <v>7525</v>

</xml_diff>

<commit_message>
final files for backup
Former-commit-id: 1bc998408b820482d75f4f92b8d5b54298f923b8
</commit_message>
<xml_diff>
--- a/New Terminals/Scripts/ConversãoDataCDC.xlsx
+++ b/New Terminals/Scripts/ConversãoDataCDC.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\105864\Documents\Millennium\New Terminals\Scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26D531A-A4F4-4477-89D0-D54D8F376828}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81762783-80E6-43F3-A66C-9F4159F07E3F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="541" xr2:uid="{B052DA09-9D1F-47DC-9B08-88E6AD2BA9C1}"/>
+    <workbookView minimized="1" xWindow="5385" yWindow="4335" windowWidth="21600" windowHeight="11265" tabRatio="541" xr2:uid="{B052DA09-9D1F-47DC-9B08-88E6AD2BA9C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Data &lt;-&gt; CDC" sheetId="2" r:id="rId1"/>
@@ -565,7 +565,7 @@
   <dimension ref="A2:G12"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -625,18 +625,18 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="9">
-        <v>44695</v>
+        <v>44713</v>
       </c>
       <c r="C5" s="3">
         <f t="shared" ref="C5:C10" si="1">IF(B5 &gt;= DATE(2001,5,1), B5-DATE(2001,5,1)+1,"Data inválida")</f>
-        <v>7684</v>
+        <v>7702</v>
       </c>
       <c r="E5" s="2">
-        <v>7528</v>
+        <v>7599</v>
       </c>
       <c r="F5" s="8">
         <f>IF(E5 &gt; 0, DATE(2001,5,1)+E5-1, "cdc inválido")</f>
-        <v>44539</v>
+        <v>44610</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -660,11 +660,11 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7" s="9">
-        <v>44497</v>
+        <v>44708</v>
       </c>
       <c r="C7" s="3">
         <f t="shared" si="1"/>
-        <v>7486</v>
+        <v>7697</v>
       </c>
       <c r="E7" s="2">
         <v>7610</v>

</xml_diff>